<commit_message>
&& - №13035 от 22.09.2024 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Andorra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53CDE89-E622-4CBC-8142-204121B3BD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF309DC-ADB1-4EE7-9C7E-C41FE52064E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7970" yWindow="1450" windowWidth="28720" windowHeight="19550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="1450" windowWidth="28720" windowHeight="19550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -1293,7 +1293,7 @@
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1784,7 +1784,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="10" t="str">
         <f t="shared" ref="J16:J17" si="2">IF(OR(AND(H16&gt;1,H16&lt;&gt;"-"),AND(I16&gt;1,I16&lt;&gt;"-")),"Can exchange","")</f>
@@ -1817,7 +1817,7 @@
         <v>4</v>
       </c>
       <c r="I17" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1876,7 +1876,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="26" t="s">
         <v>4</v>
@@ -1910,7 +1910,7 @@
         <v>4</v>
       </c>
       <c r="I20" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="10" t="str">
         <f t="shared" ref="J20:J22" si="4">IF(OR(AND(H20&gt;1,H20&lt;&gt;"-"),AND(I20&gt;1,I20&lt;&gt;"-")),"Can exchange","")</f>
@@ -1941,7 +1941,7 @@
         <v>4</v>
       </c>
       <c r="I21" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="10" t="str">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
& - №17896 от 29.04.2025 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Andorra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF309DC-ADB1-4EE7-9C7E-C41FE52064E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F21420-B4F0-4AA1-8906-F88F990800B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="1450" windowWidth="28720" windowHeight="19550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
             <charset val="204"/>
           </rPr>
           <t>Fábrica Nacional de Moneda y Timbre - Real Casa de la Moneda
-(Royal Mint of Spain)</t>
+(Royal Mint of Madrid)</t>
         </r>
       </text>
     </comment>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="51">
   <si>
     <t>Year</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>Subtype_3#Map_of_Europe</t>
+  </si>
+  <si>
+    <t>100th Anniversary - Skiing in Andorra</t>
+  </si>
+  <si>
+    <t>2024 UCI Mountain Bike World Championships</t>
   </si>
 </sst>
 </file>
@@ -777,7 +783,7 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="30">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -786,6 +792,14 @@
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1287,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1913,7 +1927,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="10" t="str">
-        <f t="shared" ref="J20:J22" si="4">IF(OR(AND(H20&gt;1,H20&lt;&gt;"-"),AND(I20&gt;1,I20&lt;&gt;"-")),"Can exchange","")</f>
+        <f t="shared" ref="J20:J23" si="4">IF(OR(AND(H20&gt;1,H20&lt;&gt;"-"),AND(I20&gt;1,I20&lt;&gt;"-")),"Can exchange","")</f>
         <v/>
       </c>
     </row>
@@ -1948,35 +1962,64 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="6">
         <v>2024</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="9" t="s">
+      <c r="B22" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="31">
+        <v>60000</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="33">
+        <v>1</v>
+      </c>
+      <c r="I22" s="34" t="s">
         <v>4</v>
       </c>
       <c r="J22" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
+        <v>2024</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="46">
+        <v>60000</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="48">
+        <v>1</v>
+      </c>
+      <c r="I23" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="10" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1990,11 +2033,45 @@
     <mergeCell ref="C1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:H5 H8:H9 H12:H13">
-    <cfRule type="containsText" dxfId="28" priority="95" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="29" priority="101" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5 H8:H9 H12:H13">
+    <cfRule type="colorScale" priority="102">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3 I6:I7 I10:I11">
+    <cfRule type="containsText" dxfId="28" priority="99" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I7 I3 I10:I11">
+    <cfRule type="colorScale" priority="100">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I15">
+    <cfRule type="containsText" dxfId="27" priority="95" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I15">
     <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2006,12 +2083,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3 I6:I7 I10:I11">
-    <cfRule type="containsText" dxfId="27" priority="93" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6:I7 I3 I10:I11">
+  <conditionalFormatting sqref="H16:H17">
+    <cfRule type="containsText" dxfId="26" priority="93" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:H17">
     <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2023,29 +2100,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I15">
-    <cfRule type="containsText" dxfId="26" priority="89" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I14))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I15">
-    <cfRule type="colorScale" priority="90">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:H17">
+  <conditionalFormatting sqref="I18:I19">
     <cfRule type="containsText" dxfId="25" priority="87" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:H17">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:I19">
     <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2057,13 +2117,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I19">
-    <cfRule type="containsText" dxfId="24" priority="81" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I19">
-    <cfRule type="colorScale" priority="82">
+  <conditionalFormatting sqref="H20:H21">
+    <cfRule type="containsText" dxfId="24" priority="85" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:H21">
+    <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2074,13 +2134,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H21">
-    <cfRule type="containsText" dxfId="23" priority="79" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H21">
-    <cfRule type="colorScale" priority="80">
+  <conditionalFormatting sqref="H6:H7">
+    <cfRule type="containsText" dxfId="23" priority="41" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H7">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2091,12 +2151,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="I5">
     <cfRule type="containsText" dxfId="22" priority="39" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I5))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2108,12 +2168,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
+  <conditionalFormatting sqref="I4">
     <cfRule type="containsText" dxfId="21" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2125,12 +2185,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H7">
+  <conditionalFormatting sqref="H3">
     <cfRule type="containsText" dxfId="20" priority="35" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H6))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H7">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2142,12 +2202,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="I8">
     <cfRule type="containsText" dxfId="19" priority="33" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I5))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2159,12 +2219,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+  <conditionalFormatting sqref="I9">
     <cfRule type="containsText" dxfId="18" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2176,12 +2236,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="H10">
     <cfRule type="containsText" dxfId="17" priority="29" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2193,12 +2253,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+  <conditionalFormatting sqref="H11">
     <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2210,12 +2270,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
+  <conditionalFormatting sqref="H14">
     <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2227,12 +2287,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="H15">
     <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2244,12 +2304,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="I12">
     <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H11))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2261,12 +2321,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+  <conditionalFormatting sqref="I13">
     <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2278,12 +2338,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="I16">
     <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2295,12 +2355,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="I17">
     <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2312,12 +2372,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
+  <conditionalFormatting sqref="H18">
     <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2329,12 +2389,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2346,12 +2406,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
+  <conditionalFormatting sqref="I20">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2363,12 +2423,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="I21">
     <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2380,12 +2440,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+  <conditionalFormatting sqref="I22:I23">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:I23">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2397,12 +2457,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+  <conditionalFormatting sqref="H22">
     <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2414,12 +2474,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="H23">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I21))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2442,7 +2502,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
&& - 19856 от 02.07.2025 https://2eurostore.ru/ - 19935 от 07.07.2025 https://2eurostore.ru/ - 80195020 от 21.07.2025 https://meshok.net/ - 80173384 от 20.07.2025 https://meshok.net/ - 80173191 от 20.07.2025 https://meshok.net/ - 80173113 от 20.07.2025 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Andorra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5F1EA-028B-485C-83B5-782467A254AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1B3468-26DE-4442-B1F6-DE2C288569EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="33150" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -1440,7 +1440,7 @@
       <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1828,7 +1828,7 @@
         <v>4</v>
       </c>
       <c r="I12" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="56"/>
       <c r="K12" s="10" t="str">

</xml_diff>